<commit_message>
Add new sheet for new bot
</commit_message>
<xml_diff>
--- a/Control.xlsx
+++ b/Control.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos Uipath\Devolucion-de-Percepcion-Ganancias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7AE172-E70F-49D6-8A66-AFE199AA8EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBC0199-43D4-4B19-A294-6C8C7E277A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="20490" windowHeight="10830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Control" sheetId="1" r:id="rId1"/>
+    <sheet name="Control Rec" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Control!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Control Rec'!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Fila</t>
   </si>
@@ -379,11 +381,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -394,7 +394,29 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:B1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D8BB92-AA6F-459C-A0C1-740AEEFBB8C6}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>